<commit_message>
Validar visualizacion de producto
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dipialeso\Documents\Entrenamiento Dirigido (ED)\Automatizacion\AutomatizacionFlujoCompraProductoOpencart\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6441D89-FEEF-4FBC-92C6-DE6A52E4924C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25DFC86-4D6F-4C07-9E19-E0126B5DAFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -438,9 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Ingreso de datos personales
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dipialeso\Documents\Entrenamiento Dirigido (ED)\Automatizacion\AutomatizacionFlujoCompraProductoOpencart\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dipialeso\Documents\ED\AutomatizacionFlujoCompraProductoOpencart\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25DFC86-4D6F-4C07-9E19-E0126B5DAFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F087CE2-E1C2-499E-8982-5AD60D8A9537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CA2474-79AA-45C0-875C-4B16A37B45E7}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>